<commit_message>
switching to BC specifics
</commit_message>
<xml_diff>
--- a/data/RAW BC_Data_100220.xlsx
+++ b/data/RAW BC_Data_100220.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lknelson\Documents\GitHub\climate_perceptions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62E357BC-0699-4F47-863E-DEBD55D02139}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C9A556-8992-43B0-81D9-4D8F4C34DE07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20760" yWindow="795" windowWidth="15555" windowHeight="14445" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A1" sheetId="1" r:id="rId1"/>
     <sheet name="Datamap" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3203" uniqueCount="2105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3257" uniqueCount="2132">
   <si>
     <t>record</t>
   </si>
@@ -6336,13 +6337,94 @@
   </si>
   <si>
     <t>[q20ar6oe]: For the next question, you will be asked what, if any, effect you believe ocean warming is having on specific fisheries. For each fishery, we would like you to indicate if you think ocean warming is having a strong or slightly negative effect, no effect, or a slightly or strongly positive effect. You many also answer I don't know. Then you will be asked about your confidence level in that answer.What, if any, effect do you believe ocean warming is having on these commercial fisheries? - Other</t>
+  </si>
+  <si>
+    <t>salmon_troll</t>
+  </si>
+  <si>
+    <t>salmon_seine</t>
+  </si>
+  <si>
+    <t>salmon_gillnet</t>
+  </si>
+  <si>
+    <t>herring_roe_gillnet</t>
+  </si>
+  <si>
+    <t>herring_roe_seine</t>
+  </si>
+  <si>
+    <t>herring_spawn_on_kelp</t>
+  </si>
+  <si>
+    <t>tuna_troll</t>
+  </si>
+  <si>
+    <t>tuna_international</t>
+  </si>
+  <si>
+    <t>tuna_us</t>
+  </si>
+  <si>
+    <t>hake_midtrawl</t>
+  </si>
+  <si>
+    <t>sardine</t>
+  </si>
+  <si>
+    <t>groundfish_trawl</t>
+  </si>
+  <si>
+    <t>halibut_longline</t>
+  </si>
+  <si>
+    <t>sablefish_longline</t>
+  </si>
+  <si>
+    <t>sablefish_trap</t>
+  </si>
+  <si>
+    <t>rockfish_hl</t>
+  </si>
+  <si>
+    <t>lingcod_hl</t>
+  </si>
+  <si>
+    <t>dogfish_hl</t>
+  </si>
+  <si>
+    <t>shrimp_trawl</t>
+  </si>
+  <si>
+    <t>euphausiid_trawl</t>
+  </si>
+  <si>
+    <t>prawn_shrimp_trap</t>
+  </si>
+  <si>
+    <t>crab_trap</t>
+  </si>
+  <si>
+    <t>geoduck_horseclam_dive</t>
+  </si>
+  <si>
+    <t>redseaurchin_dive</t>
+  </si>
+  <si>
+    <t>greenseaurchin_dive</t>
+  </si>
+  <si>
+    <t>seacucumber_dive</t>
+  </si>
+  <si>
+    <t>other</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6473,6 +6555,19 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -6819,8 +6914,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -7178,7 +7276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:JS106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="BN1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -86959,8 +87057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C670"/>
   <sheetViews>
-    <sheetView topLeftCell="A574" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -92946,4 +93044,237 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E55C4A-A255-4C6C-82F4-3E2093C67EC5}">
+  <dimension ref="B2:C28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>2105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>2106</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>2107</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>2108</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>2109</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>2110</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>2111</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>2112</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>2113</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>2114</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>2115</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>2116</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>2117</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>2118</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>2119</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>2120</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>2121</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>2122</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>2123</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>2124</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>2125</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>2126</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>2127</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>2128</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>2129</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>2130</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>